<commit_message>
feat: add participant json
</commit_message>
<xml_diff>
--- a/OCABundles/schema/credebl/participant/Participant.xlsx
+++ b/OCABundles/schema/credebl/participant/Participant.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="130">
   <si>
     <t>OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -1138,9 +1138,6 @@
     <t>full_name</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>utf-8</t>
   </si>
   <si>
@@ -2146,9 +2143,6 @@
     <xf borderId="41" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -2159,6 +2153,9 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -5462,19 +5459,17 @@
       <c r="C4" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="74" t="s">
         <v>100</v>
-      </c>
-      <c r="E4" s="75" t="s">
-        <v>101</v>
       </c>
       <c r="F4" s="71"/>
       <c r="G4" s="71"/>
       <c r="H4" s="71"/>
       <c r="I4" s="49"/>
       <c r="J4" s="71"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="77"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="76"/>
       <c r="M4" s="71"/>
       <c r="N4" s="71"/>
       <c r="O4" s="71"/>
@@ -5497,22 +5492,20 @@
         <v/>
       </c>
       <c r="B5" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="71"/>
+      <c r="E5" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="75" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="71" t="s">
         <v>103</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>104</v>
       </c>
       <c r="H5" s="71"/>
       <c r="I5" s="49"/>
@@ -5541,16 +5534,14 @@
         <v/>
       </c>
       <c r="B6" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="74" t="s">
         <v>100</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>101</v>
       </c>
       <c r="F6" s="71"/>
       <c r="G6" s="71"/>
@@ -5581,16 +5572,14 @@
         <v/>
       </c>
       <c r="B7" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="71"/>
+      <c r="E7" s="74" t="s">
         <v>100</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>101</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="71"/>
@@ -5621,16 +5610,14 @@
         <v/>
       </c>
       <c r="B8" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="71"/>
+      <c r="E8" s="74" t="s">
         <v>100</v>
-      </c>
-      <c r="E8" s="75" t="s">
-        <v>101</v>
       </c>
       <c r="F8" s="71"/>
       <c r="G8" s="71"/>
@@ -37578,10 +37565,10 @@
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="85" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="85" t="s">
         <v>108</v>
-      </c>
-      <c r="B3" s="85" t="s">
-        <v>109</v>
       </c>
       <c r="C3" s="60" t="s">
         <v>19</v>
@@ -37598,21 +37585,21 @@
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="88" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>111</v>
       </c>
       <c r="C4" s="89" t="str">
         <f>IF(ISBLANK(Main!$B4),"",Main!$B4)</f>
         <v>full_name</v>
       </c>
       <c r="D4" s="90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="91"/>
       <c r="F4" s="90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
@@ -37637,21 +37624,21 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="93" t="s">
         <v>114</v>
-      </c>
-      <c r="B5" s="93" t="s">
-        <v>115</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>IF(ISBLANK(Main!$B5),"",Main!$B5)</f>
         <v>date_of_birth</v>
       </c>
       <c r="D5" s="94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="95"/>
       <c r="F5" s="94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
@@ -37676,21 +37663,21 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="93" t="s">
         <v>118</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>119</v>
       </c>
       <c r="C6" s="71" t="str">
         <f>IF(ISBLANK(Main!$B6),"",Main!$B6)</f>
         <v>country</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E6" s="95"/>
       <c r="F6" s="94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
@@ -37715,21 +37702,21 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="96" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="71" t="str">
         <f>IF(ISBLANK(Main!$B7),"",Main!$B7)</f>
         <v>category</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="95"/>
       <c r="F7" s="94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
@@ -37754,21 +37741,21 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="96" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="98" t="s">
         <v>125</v>
-      </c>
-      <c r="B8" s="98" t="s">
-        <v>126</v>
       </c>
       <c r="C8" s="71" t="str">
         <f>IF(ISBLANK(Main!$B8),"",Main!$B8)</f>
         <v>issued_by</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="95"/>
       <c r="F8" s="94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="49"/>
@@ -37793,7 +37780,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="96" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B9" s="99"/>
       <c r="C9" s="71" t="str">
@@ -37826,10 +37813,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="71" t="str">
         <f>IF(ISBLANK(Main!$B10),"",Main!$B10)</f>

</xml_diff>

<commit_message>
refactor: add flagged attributes for participant
</commit_message>
<xml_diff>
--- a/OCABundles/schema/credebl/participant/Participant.xlsx
+++ b/OCABundles/schema/credebl/participant/Participant.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
   <si>
     <t>OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -1138,6 +1138,9 @@
     <t>full_name</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>utf-8</t>
   </si>
   <si>
@@ -2143,6 +2146,9 @@
     <xf borderId="41" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -2153,9 +2159,6 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -5459,17 +5462,19 @@
       <c r="C4" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="74" t="s">
+      <c r="D4" s="74" t="s">
         <v>100</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F4" s="71"/>
       <c r="G4" s="71"/>
       <c r="H4" s="71"/>
       <c r="I4" s="49"/>
       <c r="J4" s="71"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77"/>
       <c r="M4" s="71"/>
       <c r="N4" s="71"/>
       <c r="O4" s="71"/>
@@ -5492,20 +5497,22 @@
         <v/>
       </c>
       <c r="B5" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="74" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="78" t="s">
-        <v>102</v>
+      <c r="F5" s="74" t="s">
+        <v>103</v>
       </c>
       <c r="G5" s="71" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H5" s="71"/>
       <c r="I5" s="49"/>
@@ -5534,14 +5541,16 @@
         <v/>
       </c>
       <c r="B6" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="74" t="s">
+      <c r="D6" s="74" t="s">
         <v>100</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F6" s="71"/>
       <c r="G6" s="71"/>
@@ -5572,14 +5581,16 @@
         <v/>
       </c>
       <c r="B7" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="74" t="s">
+      <c r="D7" s="74" t="s">
         <v>100</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="71"/>
@@ -5610,14 +5621,16 @@
         <v/>
       </c>
       <c r="B8" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="74" t="s">
+      <c r="D8" s="74" t="s">
         <v>100</v>
+      </c>
+      <c r="E8" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F8" s="71"/>
       <c r="G8" s="71"/>
@@ -37565,10 +37578,10 @@
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="85" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="60" t="s">
         <v>19</v>
@@ -37585,21 +37598,21 @@
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="87" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C4" s="89" t="str">
         <f>IF(ISBLANK(Main!$B4),"",Main!$B4)</f>
         <v>full_name</v>
       </c>
       <c r="D4" s="90" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E4" s="91"/>
       <c r="F4" s="90" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
@@ -37624,21 +37637,21 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="92" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B5" s="93" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>IF(ISBLANK(Main!$B5),"",Main!$B5)</f>
         <v>date_of_birth</v>
       </c>
       <c r="D5" s="94" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E5" s="95"/>
       <c r="F5" s="94" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
@@ -37663,21 +37676,21 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="96" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="71" t="str">
         <f>IF(ISBLANK(Main!$B6),"",Main!$B6)</f>
         <v>country</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E6" s="95"/>
       <c r="F6" s="94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
@@ -37702,21 +37715,21 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="96" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="71" t="str">
         <f>IF(ISBLANK(Main!$B7),"",Main!$B7)</f>
         <v>category</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E7" s="95"/>
       <c r="F7" s="94" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
@@ -37741,21 +37754,21 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="96" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C8" s="71" t="str">
         <f>IF(ISBLANK(Main!$B8),"",Main!$B8)</f>
         <v>issued_by</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E8" s="95"/>
       <c r="F8" s="94" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="49"/>
@@ -37780,7 +37793,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="96" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" s="99"/>
       <c r="C9" s="71" t="str">
@@ -37813,10 +37826,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="96" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C10" s="71" t="str">
         <f>IF(ISBLANK(Main!$B10),"",Main!$B10)</f>

</xml_diff>